<commit_message>
SQL class, loans and payments
</commit_message>
<xml_diff>
--- a/tablas/deudores.xlsx
+++ b/tablas/deudores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidbedoya/Documents/Repositories/inversiones/tablas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250B2B6F-CCF3-7C4F-9480-434E7552AC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9CEBFA-63BB-1E4C-A4FA-57160780081C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{CD76133A-3D91-B24D-8AAB-CE950D21A176}"/>
+    <workbookView xWindow="9240" yWindow="1480" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{CD76133A-3D91-B24D-8AAB-CE950D21A176}"/>
   </bookViews>
   <sheets>
     <sheet name="DEUDORES" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="ABONOS" sheetId="3" r:id="rId3"/>
     <sheet name="CONTABILIDAD" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>HIP</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>INCREMENTAL</t>
   </si>
   <si>
     <t>28/06/2022</t>
@@ -110,7 +107,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -227,33 +224,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -569,153 +564,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26CF11E4-1266-314D-91CD-CF6709615CFA}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" customWidth="1"/>
-    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1622</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3">
+        <v>123</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="8">
+        <v>23000000</v>
+      </c>
+      <c r="G2" s="9">
+        <v>7000000</v>
+      </c>
+      <c r="H2" s="9">
+        <v>2000000</v>
+      </c>
+      <c r="I2" s="7">
+        <f>SUM(F2:H2)</f>
+        <v>32000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2848</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
+        <v>456</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="9">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1622</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3">
-        <v>123</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="7">
-        <v>40000000</v>
-      </c>
-      <c r="H2" s="8">
-        <v>23000000</v>
-      </c>
-      <c r="I2" s="9">
-        <v>7000000</v>
-      </c>
-      <c r="J2" s="9">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2848</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3">
-        <v>456</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="10">
-        <v>20000000</v>
+      <c r="G3" s="9">
+        <v>0</v>
       </c>
       <c r="H3" s="9">
         <v>0</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="7">
+        <f t="shared" ref="I3:I4" si="0">SUM(F3:H3)</f>
         <v>0</v>
       </c>
-      <c r="J3" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>2652</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3">
+      <c r="C4" s="3">
         <v>789</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="7">
-        <f t="shared" ref="G4" si="0">SUM(H4:J4)</f>
+      <c r="F4" s="8">
+        <v>15000000</v>
+      </c>
+      <c r="G4" s="9">
+        <v>1000000</v>
+      </c>
+      <c r="H4" s="9">
+        <v>1000000</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="0"/>
         <v>17000000</v>
-      </c>
-      <c r="H4" s="8">
-        <v>15000000</v>
-      </c>
-      <c r="I4" s="9">
-        <v>1000000</v>
-      </c>
-      <c r="J4" s="9">
-        <v>1000000</v>
       </c>
     </row>
   </sheetData>
@@ -725,10 +709,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33016C06-EE4B-E74F-A9B3-0C51AE163353}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,32 +720,34 @@
     <col min="2" max="2" width="10.83203125" style="6"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
@@ -770,11 +756,48 @@
       <c r="B2" s="3">
         <v>123</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="14">
         <v>45107</v>
       </c>
       <c r="D2" s="7">
         <v>640000</v>
+      </c>
+      <c r="E2" s="15">
+        <f>E4*D2</f>
+        <v>460000</v>
+      </c>
+      <c r="F2" s="15">
+        <f>F4*D2</f>
+        <v>140000</v>
+      </c>
+      <c r="G2" s="15">
+        <f>G4*D2</f>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>32000000</v>
+      </c>
+      <c r="F3">
+        <v>32000000</v>
+      </c>
+      <c r="G3">
+        <v>32000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <f>DEUDORES!F2/E3</f>
+        <v>0.71875</v>
+      </c>
+      <c r="F4">
+        <f>DEUDORES!G2/F3</f>
+        <v>0.21875</v>
+      </c>
+      <c r="G4">
+        <f>DEUDORES!H2/G3</f>
+        <v>6.25E-2</v>
       </c>
     </row>
   </sheetData>
@@ -796,17 +819,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -816,19 +839,19 @@
       <c r="B2" s="3">
         <v>123</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="14">
         <v>45107</v>
       </c>
       <c r="D2" s="7">
         <v>640000</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{387961BE-73C0-8D4D-8433-A179512AD499}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>